<commit_message>
Login feature ,stepdefinition and pageobject class
</commit_message>
<xml_diff>
--- a/target/test-classes/TestData/ExcelData.xlsx
+++ b/target/test-classes/TestData/ExcelData.xlsx
@@ -1,11 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{27BA8E87-001B-4DFB-BDAF-7CBAD7E75E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jithu\git\Team01_ActionSquad\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9960"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="12" r:id="rId1"/>
@@ -13,13 +17,12 @@
     <sheet name="Batch" sheetId="10" r:id="rId3"/>
     <sheet name="Class" sheetId="11" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:O29"/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>username</t>
   </si>
@@ -30,6 +33,21 @@
     <t>message</t>
   </si>
   <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
     <t>sdetnumpyninja@gmail.com</t>
   </si>
   <si>
@@ -39,9 +57,75 @@
     <t>LMS - Learning Management System</t>
   </si>
   <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Staff Data</t>
+  </si>
+  <si>
+    <t>Manage User</t>
+  </si>
+  <si>
+    <t>Sdet</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Invalid username and password.Please try again</t>
+  </si>
+  <si>
+    <t>LMS</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Manage Batch</t>
+  </si>
+  <si>
+    <t>Invalid test case input</t>
+  </si>
+  <si>
+    <t>Batch</t>
+  </si>
+  <si>
+    <t>Batches</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
     <t>Manage Program</t>
   </si>
   <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Programs</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Headers</t>
+  </si>
+  <si>
     <t>Program Name</t>
   </si>
   <si>
@@ -54,83 +138,14 @@
     <t>Add New Program</t>
   </si>
   <si>
-    <t>Headers</t>
-  </si>
-  <si>
-    <t>Home</t>
-  </si>
-  <si>
-    <t>Program</t>
-  </si>
-  <si>
-    <t>Batch</t>
-  </si>
-  <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>Logout</t>
-  </si>
-  <si>
     <t>Edit / Delete</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>menu</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>table</t>
-  </si>
-  <si>
-    <t>page</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>Staff Data</t>
-  </si>
-  <si>
-    <t>Manage User</t>
-  </si>
-  <si>
-    <t>LMS</t>
-  </si>
-  <si>
-    <t>Staff</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>Manage Batch</t>
-  </si>
-  <si>
-    <t>Batches</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Programs</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Phone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,17 +154,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -162,39 +170,24 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -203,10 +196,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -372,6 +365,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -395,10 +389,11 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -407,13 +402,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="25400" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -489,6 +484,7 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -508,264 +504,271 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A01634-65B9-471D-B1E1-B2B81A92F07E}">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.109375" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" customWidth="1"/>
+    <col min="1" max="1" width="26.28516" customWidth="1"/>
+    <col min="2" max="2" width="16.42578" customWidth="1"/>
+    <col min="3" max="3" width="30.71094" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
+    <row r="4">
+      <c r="A4"/>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="D4"/>
+      <c r="E4" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="F4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
+      <c r="G4" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="H4" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="1" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5"/>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="F5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="G5" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H5"/>
+    </row>
+    <row r="6">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="F6"/>
+      <c r="G6" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="1"/>
+      <c r="H6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{61904FCD-2F64-48BD-AC72-3C27C9D86959}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5673E90-C4D8-4E19-B448-4406659E4150}">
-  <dimension ref="A1:A13"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="1" max="1" width="28.66406" customWidth="1"/>
     <col min="2" max="2" width="15.21875" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="19.77734" customWidth="1"/>
     <col min="5" max="5" width="19.21875" customWidth="1"/>
-    <col min="6" max="6" width="16.77734375" customWidth="1"/>
+    <col min="6" max="6" width="16.77734" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4">
       <c r="A4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB0D9E38-544C-414C-8631-AA4FAACA7E16}">
-  <dimension ref="A1"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{734070C0-1B6A-4792-849F-EBC031903E15}">
-  <dimension ref="A1"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>